<commit_message>
Morada” should stop at the beginning of the postal code and not include it (Avenida Capitão António Gomes da Rocha, Nº 14, 5º A, Monte Abraão 2745-246 Queluz)
</commit_message>
<xml_diff>
--- a/webscrapping school/msaces/racius_links_output.xlsx
+++ b/webscrapping school/msaces/racius_links_output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S59"/>
+  <dimension ref="A1:S40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1107,7 +1107,7 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>Rua Cidade de Córdova, 2A 2610-038 Amadora</t>
+          <t>Rua Cidade de Córdova, 2A</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
@@ -1186,7 +1186,7 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>Rua da Ermida, N.º 64 4465-126 S. Mamede de Infesta</t>
+          <t>Rua da Ermida, N.º 64</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
@@ -1720,7 +1720,7 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>Rua Ana de Castro Osório, Nº 2 C 1500-023 Lisboa</t>
+          <t>Rua Ana de Castro Osório, Nº 2 C</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
@@ -2254,7 +2254,7 @@
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>Rua António Bessa Leite, 1468, Loja 11, Porto 4150-077 Porto</t>
+          <t>Rua António Bessa Leite, 1468, Loja 11, Porto</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
@@ -2337,7 +2337,7 @@
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>Rua da Reserva Botânica, Número 11, Garagem 4, Rinchoa 2635-460 Rio de Mouro</t>
+          <t>Rua da Reserva Botânica, Número 11, Garagem 4, Rinchoa</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
@@ -2420,7 +2420,7 @@
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>Rua Gago Coutinho e Sacadura Cabral, Nº 21/21A/21B 2955-210 Pinhal Novo</t>
+          <t>Rua Gago Coutinho e Sacadura Cabral, Nº 21/21A/21B</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
@@ -2594,7 +2594,7 @@
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>Rua das Passarias, Nº 251 4445-171 Alfena</t>
+          <t>Rua das Passarias, Nº 251</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
@@ -2764,7 +2764,7 @@
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>Rua Manuel Teixeira Gomes, Nº. 22, 1º., Dtº. 2790-103 Carnaxide</t>
+          <t>Rua Manuel Teixeira Gomes, Nº. 22, 1º., Dtº.</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
@@ -3959,1689 +3959,6 @@
         </is>
       </c>
     </row>
-    <row r="41">
-      <c r="A41" t="inlineStr">
-        <is>
-          <t>747680</t>
-        </is>
-      </c>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>2025.06.11</t>
-        </is>
-      </c>
-      <c r="C41" t="inlineStr">
-        <is>
-          <t>FIEIS AOS TACHOS, LDA</t>
-        </is>
-      </c>
-      <c r="D41" t="n">
-        <v>25</v>
-      </c>
-      <c r="E41" t="inlineStr"/>
-      <c r="F41" t="inlineStr">
-        <is>
-          <t>(531)  27.5.13</t>
-        </is>
-      </c>
-      <c r="G41" t="inlineStr">
-        <is>
-          <t>https://www.racius.com/fieis-aos-tachos-lda/</t>
-        </is>
-      </c>
-      <c r="H41" t="inlineStr">
-        <is>
-          <t>516856197</t>
-        </is>
-      </c>
-      <c r="I41" t="inlineStr">
-        <is>
-          <t>Travessa dos Mastros, Nº 25 1200-337 Lisboa</t>
-        </is>
-      </c>
-      <c r="J41" t="inlineStr">
-        <is>
-          <t>1200-337</t>
-        </is>
-      </c>
-      <c r="K41" t="inlineStr">
-        <is>
-          <t>06/2025</t>
-        </is>
-      </c>
-      <c r="L41" t="inlineStr">
-        <is>
-          <t>06/2035</t>
-        </is>
-      </c>
-      <c r="M41" t="inlineStr">
-        <is>
-          <t>2025-06-30</t>
-        </is>
-      </c>
-      <c r="N41" t="n">
-        <v>0</v>
-      </c>
-      <c r="O41" t="n">
-        <v>0</v>
-      </c>
-      <c r="P41" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q41" t="n">
-        <v>0</v>
-      </c>
-      <c r="R41" t="inlineStr">
-        <is>
-          <t>123456798</t>
-        </is>
-      </c>
-      <c r="S41" t="inlineStr">
-        <is>
-          <t>12354</t>
-        </is>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t>747681</t>
-        </is>
-      </c>
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>2025.06.11</t>
-        </is>
-      </c>
-      <c r="C42" t="inlineStr">
-        <is>
-          <t>MOBSTER LDA</t>
-        </is>
-      </c>
-      <c r="D42" t="n">
-        <v>35</v>
-      </c>
-      <c r="E42" t="inlineStr"/>
-      <c r="F42" t="inlineStr">
-        <is>
-          <t>(531)  27.5.10 ; 27.5.17</t>
-        </is>
-      </c>
-      <c r="G42" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="H42" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="I42" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="J42" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="K42" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="L42" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="M42" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="N42" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="O42" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="P42" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="Q42" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="R42" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="S42" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>747682</t>
-        </is>
-      </c>
-      <c r="B43" t="inlineStr">
-        <is>
-          <t>2025.06.11</t>
-        </is>
-      </c>
-      <c r="C43" t="inlineStr">
-        <is>
-          <t>CRISTIANO DAVID CAMACHO RODRIGUES ABREU</t>
-        </is>
-      </c>
-      <c r="D43" t="n">
-        <v>35</v>
-      </c>
-      <c r="E43" t="inlineStr"/>
-      <c r="F43" t="inlineStr">
-        <is>
-          <t>(531)  27.99.3</t>
-        </is>
-      </c>
-      <c r="G43" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="H43" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="I43" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="J43" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="K43" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="L43" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="M43" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="N43" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="O43" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="P43" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="Q43" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="R43" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="S43" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>747683</t>
-        </is>
-      </c>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>2025.06.11</t>
-        </is>
-      </c>
-      <c r="C44" t="inlineStr">
-        <is>
-          <t>MOBSTER LDA</t>
-        </is>
-      </c>
-      <c r="D44" t="n">
-        <v>35</v>
-      </c>
-      <c r="E44" t="inlineStr">
-        <is>
-          <t>BOLETIM DA PROPRIEDADE INDUSTRIAL N.º 2025/06/30</t>
-        </is>
-      </c>
-      <c r="F44" t="inlineStr"/>
-      <c r="G44" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="H44" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="I44" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="J44" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="K44" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="L44" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="M44" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="N44" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="O44" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="P44" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="Q44" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="R44" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="S44" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t>747684</t>
-        </is>
-      </c>
-      <c r="B45" t="inlineStr">
-        <is>
-          <t>2025.06.11</t>
-        </is>
-      </c>
-      <c r="C45" t="inlineStr">
-        <is>
-          <t>LUCIA MARIA PINHEIRO DOS SANTOS</t>
-        </is>
-      </c>
-      <c r="D45" t="n">
-        <v>41</v>
-      </c>
-      <c r="E45" t="inlineStr">
-        <is>
-          <t>MNA</t>
-        </is>
-      </c>
-      <c r="F45" t="inlineStr"/>
-      <c r="G45" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="H45" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="I45" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="J45" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="K45" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="L45" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="M45" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="N45" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="O45" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="P45" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="Q45" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="R45" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="S45" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t>747687</t>
-        </is>
-      </c>
-      <c r="B46" t="inlineStr">
-        <is>
-          <t>2025.06.11</t>
-        </is>
-      </c>
-      <c r="C46" t="inlineStr">
-        <is>
-          <t>MYMETRO - CONSULTING, TRAINING</t>
-        </is>
-      </c>
-      <c r="D46" t="n">
-        <v>41</v>
-      </c>
-      <c r="E46" t="inlineStr"/>
-      <c r="F46" t="inlineStr"/>
-      <c r="G46" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="H46" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="I46" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="J46" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="K46" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="L46" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="M46" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="N46" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="O46" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="P46" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="Q46" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="R46" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="S46" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="inlineStr">
-        <is>
-          <t>747685</t>
-        </is>
-      </c>
-      <c r="B47" t="inlineStr">
-        <is>
-          <t>2025.06.11</t>
-        </is>
-      </c>
-      <c r="C47" t="inlineStr">
-        <is>
-          <t>MYMETRO - CONSULTING, TRAINING</t>
-        </is>
-      </c>
-      <c r="D47" t="n">
-        <v>41</v>
-      </c>
-      <c r="E47" t="inlineStr"/>
-      <c r="F47" t="inlineStr">
-        <is>
-          <t>(531)  26.1.5 ; 26.99.6</t>
-        </is>
-      </c>
-      <c r="G47" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="H47" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="I47" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="J47" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="K47" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="L47" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="M47" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="N47" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="O47" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="P47" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="Q47" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="R47" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="S47" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="inlineStr">
-        <is>
-          <t>747696</t>
-        </is>
-      </c>
-      <c r="B48" t="inlineStr">
-        <is>
-          <t>2025.06.11</t>
-        </is>
-      </c>
-      <c r="C48" t="inlineStr">
-        <is>
-          <t>PAULO ROBERTO GARRIDO MACEDO</t>
-        </is>
-      </c>
-      <c r="D48" t="n">
-        <v>5</v>
-      </c>
-      <c r="E48" t="inlineStr"/>
-      <c r="F48" t="inlineStr"/>
-      <c r="G48" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="H48" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="I48" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="J48" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="K48" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="L48" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="M48" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="N48" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="O48" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="P48" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="Q48" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="R48" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="S48" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="inlineStr">
-        <is>
-          <t>747686</t>
-        </is>
-      </c>
-      <c r="B49" t="inlineStr">
-        <is>
-          <t>2025.06.11</t>
-        </is>
-      </c>
-      <c r="C49" t="inlineStr">
-        <is>
-          <t>MYMETRO - CONSULTING, TRAINING</t>
-        </is>
-      </c>
-      <c r="D49" t="n">
-        <v>35</v>
-      </c>
-      <c r="E49" t="inlineStr"/>
-      <c r="F49" t="inlineStr"/>
-      <c r="G49" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="H49" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="I49" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="J49" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="K49" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="L49" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="M49" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="N49" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="O49" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="P49" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="Q49" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="R49" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="S49" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="inlineStr">
-        <is>
-          <t>747834</t>
-        </is>
-      </c>
-      <c r="B50" t="inlineStr">
-        <is>
-          <t>2025.05.26</t>
-        </is>
-      </c>
-      <c r="C50" t="inlineStr">
-        <is>
-          <t>NEVES FERREIRA, ROCHA ALVES &amp;</t>
-        </is>
-      </c>
-      <c r="D50" t="n">
-        <v>41</v>
-      </c>
-      <c r="E50" t="inlineStr"/>
-      <c r="F50" t="inlineStr">
-        <is>
-          <t>(531)  27.5.1</t>
-        </is>
-      </c>
-      <c r="G50" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="H50" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="I50" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="J50" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="K50" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="L50" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="M50" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="N50" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="O50" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="P50" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="Q50" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="R50" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="S50" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="inlineStr">
-        <is>
-          <t>58103</t>
-        </is>
-      </c>
-      <c r="B51" t="inlineStr">
-        <is>
-          <t>2025.05.07</t>
-        </is>
-      </c>
-      <c r="C51" t="inlineStr">
-        <is>
-          <t>HELDER MADEIRA LIMA AFONSO</t>
-        </is>
-      </c>
-      <c r="D51" t="inlineStr"/>
-      <c r="E51" t="inlineStr"/>
-      <c r="F51" t="inlineStr"/>
-      <c r="G51" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="H51" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="I51" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="J51" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="K51" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="L51" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="M51" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="N51" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="O51" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="P51" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="Q51" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="R51" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="S51" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="inlineStr">
-        <is>
-          <t>58208</t>
-        </is>
-      </c>
-      <c r="B52" t="inlineStr">
-        <is>
-          <t>2025.06.09</t>
-        </is>
-      </c>
-      <c r="C52" t="inlineStr">
-        <is>
-          <t>MÁRIO RUI VELHIO MODESTO</t>
-        </is>
-      </c>
-      <c r="D52" t="inlineStr"/>
-      <c r="E52" t="inlineStr">
-        <is>
-          <t>E OUTRAS ATIVIDADES RECREATIVAS</t>
-        </is>
-      </c>
-      <c r="F52" t="inlineStr"/>
-      <c r="G52" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="H52" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="I52" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="J52" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="K52" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="L52" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="M52" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="N52" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="O52" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="P52" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="Q52" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="R52" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="S52" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="inlineStr">
-        <is>
-          <t>58205</t>
-        </is>
-      </c>
-      <c r="B53" t="inlineStr">
-        <is>
-          <t>2025.06.09</t>
-        </is>
-      </c>
-      <c r="C53" t="inlineStr">
-        <is>
-          <t>ELECTRO PORTELA &amp; COSTA LDA.</t>
-        </is>
-      </c>
-      <c r="D53" t="inlineStr"/>
-      <c r="E53" t="inlineStr"/>
-      <c r="F53" t="inlineStr">
-        <is>
-          <t>(531)  2.3.8 ; 26.13.1 ; 29.1.13</t>
-        </is>
-      </c>
-      <c r="G53" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="H53" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="I53" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="J53" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="K53" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="L53" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="M53" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="N53" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="O53" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="P53" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="Q53" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="R53" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="S53" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="inlineStr">
-        <is>
-          <t>58209</t>
-        </is>
-      </c>
-      <c r="B54" t="inlineStr">
-        <is>
-          <t>2025.06.10</t>
-        </is>
-      </c>
-      <c r="C54" t="inlineStr">
-        <is>
-          <t>FREDBRAND COMUNICAÇÃO, UNIPESSOAL, LDA. LOG</t>
-        </is>
-      </c>
-      <c r="D54" t="inlineStr"/>
-      <c r="E54" t="inlineStr">
-        <is>
-          <t>70210 - RELAÇÕES PÚBLICAS E COMUNICAÇÃO; 58140 -</t>
-        </is>
-      </c>
-      <c r="F54" t="inlineStr"/>
-      <c r="G54" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="H54" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="I54" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="J54" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="K54" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="L54" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="M54" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="N54" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="O54" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="P54" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="Q54" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="R54" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="S54" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="inlineStr">
-        <is>
-          <t>58213</t>
-        </is>
-      </c>
-      <c r="B55" t="inlineStr">
-        <is>
-          <t>2025.06.11</t>
-        </is>
-      </c>
-      <c r="C55" t="inlineStr">
-        <is>
-          <t>MYMETRO - CONSULTING, TRAINING LOG &amp; METROLOGY LDA</t>
-        </is>
-      </c>
-      <c r="D55" t="inlineStr"/>
-      <c r="E55" t="inlineStr"/>
-      <c r="F55" t="inlineStr"/>
-      <c r="G55" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="H55" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="I55" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="J55" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="K55" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="L55" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="M55" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="N55" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="O55" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="P55" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="Q55" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="R55" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="S55" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="inlineStr">
-        <is>
-          <t>58210</t>
-        </is>
-      </c>
-      <c r="B56" t="inlineStr">
-        <is>
-          <t>2025.06.10</t>
-        </is>
-      </c>
-      <c r="C56" t="inlineStr">
-        <is>
-          <t>VITRINDUSTRIA UNIPESSOAL, LDA</t>
-        </is>
-      </c>
-      <c r="D56" t="inlineStr"/>
-      <c r="E56" t="inlineStr"/>
-      <c r="F56" t="inlineStr">
-        <is>
-          <t>(531)  3.7.10 ; 3.7.16</t>
-        </is>
-      </c>
-      <c r="G56" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="H56" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="I56" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="J56" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="K56" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="L56" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="M56" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="N56" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="O56" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="P56" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="Q56" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="R56" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="S56" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="inlineStr">
-        <is>
-          <t>58212</t>
-        </is>
-      </c>
-      <c r="B57" t="inlineStr">
-        <is>
-          <t>2025.06.11</t>
-        </is>
-      </c>
-      <c r="C57" t="inlineStr">
-        <is>
-          <t>SIMAS OEIRAS E AMADORA</t>
-        </is>
-      </c>
-      <c r="D57" t="inlineStr"/>
-      <c r="E57" t="inlineStr"/>
-      <c r="F57" t="inlineStr">
-        <is>
-          <t>(531)  26.1.5 ; 26.99.6</t>
-        </is>
-      </c>
-      <c r="G57" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="H57" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="I57" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="J57" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="K57" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="L57" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="M57" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="N57" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="O57" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="P57" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="Q57" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="R57" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="S57" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="inlineStr">
-        <is>
-          <t>58214</t>
-        </is>
-      </c>
-      <c r="B58" t="inlineStr">
-        <is>
-          <t>2025.06.11</t>
-        </is>
-      </c>
-      <c r="C58" t="inlineStr">
-        <is>
-          <t>MYMETRO - CONSULTING, TRAINING LOG &amp; METROLOGY LDA</t>
-        </is>
-      </c>
-      <c r="D58" t="inlineStr"/>
-      <c r="E58" t="inlineStr">
-        <is>
-          <t>LOG</t>
-        </is>
-      </c>
-      <c r="F58" t="inlineStr"/>
-      <c r="G58" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="H58" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="I58" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="J58" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="K58" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="L58" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="M58" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="N58" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="O58" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="P58" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="Q58" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="R58" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="S58" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" t="inlineStr">
-        <is>
-          <t>58215</t>
-        </is>
-      </c>
-      <c r="B59" t="inlineStr">
-        <is>
-          <t>2025.06.11</t>
-        </is>
-      </c>
-      <c r="C59" t="inlineStr">
-        <is>
-          <t>MYMETRO - CONSULTING, TRAINING LOG &amp; METROLOGY LDA</t>
-        </is>
-      </c>
-      <c r="D59" t="inlineStr"/>
-      <c r="E59" t="inlineStr"/>
-      <c r="F59" t="inlineStr">
-        <is>
-          <t>(531)  26.1.5 ; 26.99.6</t>
-        </is>
-      </c>
-      <c r="G59" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="H59" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="I59" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="J59" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="K59" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="L59" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="M59" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="N59" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="O59" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="P59" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="Q59" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="R59" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="S59" t="inlineStr">
-        <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
– “CodigoPostal” should have number and city name (2745-246 Queluz)
</commit_message>
<xml_diff>
--- a/webscrapping school/msaces/racius_links_output.xlsx
+++ b/webscrapping school/msaces/racius_links_output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S40"/>
+  <dimension ref="A1:S59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1112,7 +1112,7 @@
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>2610-038</t>
+          <t>2610-038 Amadora</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
@@ -1191,7 +1191,7 @@
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>4465-126</t>
+          <t>4465-126 S</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
@@ -1725,7 +1725,7 @@
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>1500-023</t>
+          <t>1500-023 Lisboa</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
@@ -2259,7 +2259,7 @@
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>4150-077</t>
+          <t>4150-077 Porto</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
@@ -2342,7 +2342,7 @@
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>2635-460</t>
+          <t>2635-460 Rio de Mouro</t>
         </is>
       </c>
       <c r="K22" t="inlineStr">
@@ -2425,7 +2425,7 @@
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>2955-210</t>
+          <t>2955-210 Pinhal Novo</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
@@ -2599,7 +2599,7 @@
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>4445-171</t>
+          <t>4445-171 Alfena</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
@@ -2769,7 +2769,7 @@
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>2790-103</t>
+          <t>2790-103 Carnaxide</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
@@ -3959,6 +3959,1689 @@
         </is>
       </c>
     </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>747680</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>2025.06.11</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>FIEIS AOS TACHOS, LDA</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>25</v>
+      </c>
+      <c r="E41" t="inlineStr"/>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>(531)  27.5.13</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>https://www.racius.com/fieis-aos-tachos-lda/</t>
+        </is>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>516856197</t>
+        </is>
+      </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>Travessa dos Mastros, Nº 25</t>
+        </is>
+      </c>
+      <c r="J41" t="inlineStr">
+        <is>
+          <t>1200-337 Lisboa</t>
+        </is>
+      </c>
+      <c r="K41" t="inlineStr">
+        <is>
+          <t>06/2025</t>
+        </is>
+      </c>
+      <c r="L41" t="inlineStr">
+        <is>
+          <t>06/2035</t>
+        </is>
+      </c>
+      <c r="M41" t="inlineStr">
+        <is>
+          <t>2025-06-30</t>
+        </is>
+      </c>
+      <c r="N41" t="n">
+        <v>0</v>
+      </c>
+      <c r="O41" t="n">
+        <v>0</v>
+      </c>
+      <c r="P41" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q41" t="n">
+        <v>0</v>
+      </c>
+      <c r="R41" t="inlineStr">
+        <is>
+          <t>123456798</t>
+        </is>
+      </c>
+      <c r="S41" t="inlineStr">
+        <is>
+          <t>12354</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>747681</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>2025.06.11</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>MOBSTER LDA</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>35</v>
+      </c>
+      <c r="E42" t="inlineStr"/>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>(531)  27.5.10 ; 27.5.17</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="J42" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="K42" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="L42" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="M42" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="N42" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="O42" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="P42" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="Q42" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="R42" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="S42" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>747682</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>2025.06.11</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>CRISTIANO DAVID CAMACHO RODRIGUES ABREU</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>35</v>
+      </c>
+      <c r="E43" t="inlineStr"/>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>(531)  27.99.3</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="J43" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="K43" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="L43" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="M43" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="N43" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="O43" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="P43" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="Q43" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="R43" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="S43" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>747683</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>2025.06.11</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>MOBSTER LDA</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>35</v>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>BOLETIM DA PROPRIEDADE INDUSTRIAL N.º 2025/06/30</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr"/>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="J44" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="K44" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="L44" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="M44" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="N44" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="O44" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="P44" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="Q44" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="R44" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="S44" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>747684</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>2025.06.11</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>LUCIA MARIA PINHEIRO DOS SANTOS</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>41</v>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>MNA</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr"/>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="J45" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="K45" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="L45" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="M45" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="N45" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="O45" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="P45" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="Q45" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="R45" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="S45" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>747687</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>2025.06.11</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>MYMETRO - CONSULTING, TRAINING</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>41</v>
+      </c>
+      <c r="E46" t="inlineStr"/>
+      <c r="F46" t="inlineStr"/>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="J46" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="K46" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="L46" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="M46" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="N46" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="O46" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="P46" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="Q46" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="R46" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="S46" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>747685</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>2025.06.11</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>MYMETRO - CONSULTING, TRAINING</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>41</v>
+      </c>
+      <c r="E47" t="inlineStr"/>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>(531)  26.1.5 ; 26.99.6</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="J47" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="K47" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="L47" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="M47" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="N47" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="O47" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="P47" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="Q47" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="R47" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="S47" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>747696</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>2025.06.11</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>PAULO ROBERTO GARRIDO MACEDO</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
+        <v>5</v>
+      </c>
+      <c r="E48" t="inlineStr"/>
+      <c r="F48" t="inlineStr"/>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="J48" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="K48" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="L48" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="M48" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="N48" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="O48" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="P48" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="Q48" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="R48" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="S48" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>747686</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>2025.06.11</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>MYMETRO - CONSULTING, TRAINING</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>35</v>
+      </c>
+      <c r="E49" t="inlineStr"/>
+      <c r="F49" t="inlineStr"/>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="J49" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="K49" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="L49" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="M49" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="N49" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="O49" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="P49" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="Q49" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="R49" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="S49" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>747834</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>2025.05.26</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>NEVES FERREIRA, ROCHA ALVES &amp;</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>41</v>
+      </c>
+      <c r="E50" t="inlineStr"/>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>(531)  27.5.1</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="I50" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="J50" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="K50" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="L50" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="M50" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="N50" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="O50" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="P50" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="Q50" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="R50" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="S50" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>58103</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>2025.05.07</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>HELDER MADEIRA LIMA AFONSO</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr"/>
+      <c r="E51" t="inlineStr"/>
+      <c r="F51" t="inlineStr"/>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="I51" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="J51" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="K51" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="L51" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="M51" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="N51" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="O51" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="P51" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="Q51" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="R51" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="S51" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>58208</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>2025.06.09</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>MÁRIO RUI VELHIO MODESTO</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr"/>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>E OUTRAS ATIVIDADES RECREATIVAS</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr"/>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="I52" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="J52" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="K52" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="L52" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="M52" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="N52" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="O52" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="P52" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="Q52" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="R52" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="S52" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>58205</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>2025.06.09</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>ELECTRO PORTELA &amp; COSTA LDA.</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr"/>
+      <c r="E53" t="inlineStr"/>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>(531)  2.3.8 ; 26.13.1 ; 29.1.13</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="I53" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="J53" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="K53" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="L53" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="M53" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="N53" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="O53" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="P53" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="Q53" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="R53" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="S53" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>58209</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>2025.06.10</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>FREDBRAND COMUNICAÇÃO, UNIPESSOAL, LDA. LOG</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr"/>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>70210 - RELAÇÕES PÚBLICAS E COMUNICAÇÃO; 58140 -</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr"/>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="I54" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="J54" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="K54" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="L54" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="M54" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="N54" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="O54" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="P54" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="Q54" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="R54" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="S54" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>58213</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>2025.06.11</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>MYMETRO - CONSULTING, TRAINING LOG &amp; METROLOGY LDA</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr"/>
+      <c r="E55" t="inlineStr"/>
+      <c r="F55" t="inlineStr"/>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="I55" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="J55" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="K55" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="L55" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="M55" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="N55" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="O55" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="P55" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="Q55" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="R55" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="S55" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>58210</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>2025.06.10</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>VITRINDUSTRIA UNIPESSOAL, LDA</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr"/>
+      <c r="E56" t="inlineStr"/>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>(531)  3.7.10 ; 3.7.16</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="I56" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="J56" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="K56" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="L56" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="M56" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="N56" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="O56" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="P56" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="Q56" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="R56" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="S56" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>58212</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>2025.06.11</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>SIMAS OEIRAS E AMADORA</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr"/>
+      <c r="E57" t="inlineStr"/>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>(531)  26.1.5 ; 26.99.6</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="I57" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="J57" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="K57" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="L57" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="M57" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="N57" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="O57" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="P57" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="Q57" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="R57" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="S57" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>58214</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>2025.06.11</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>MYMETRO - CONSULTING, TRAINING LOG &amp; METROLOGY LDA</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr"/>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>LOG</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr"/>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="I58" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="J58" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="K58" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="L58" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="M58" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="N58" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="O58" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="P58" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="Q58" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="R58" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="S58" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>58215</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>2025.06.11</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>MYMETRO - CONSULTING, TRAINING LOG &amp; METROLOGY LDA</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr"/>
+      <c r="E59" t="inlineStr"/>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>(531)  26.1.5 ; 26.99.6</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="I59" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="J59" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="K59" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="L59" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="M59" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="N59" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="O59" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="P59" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="Q59" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="R59" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="S59" t="inlineStr">
+        <is>
+          <t>Not Found</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>